<commit_message>
My god, its getting beautiful
</commit_message>
<xml_diff>
--- a/NewReferences.xlsx
+++ b/NewReferences.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="101">
   <si>
     <t>Item</t>
   </si>
@@ -324,6 +324,9 @@
   </si>
   <si>
     <t>http://www.archibaseplanet.com/download/77201542.html</t>
+  </si>
+  <si>
+    <t>Modeled</t>
   </si>
 </sst>
 </file>
@@ -425,7 +428,10 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="14">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -482,13 +488,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>16</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>495300</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>82924</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
+      <xdr:col>25</xdr:col>
       <xdr:colOff>91439</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
@@ -539,20 +545,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:O46" totalsRowShown="0" headerRowDxfId="12">
-  <autoFilter ref="A1:O46"/>
-  <sortState ref="A2:O46">
-    <sortCondition ref="F1:F46"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:P46" totalsRowShown="0" headerRowDxfId="13">
+  <autoFilter ref="A1:P46"/>
+  <sortState ref="A2:P46">
+    <sortCondition ref="G1:G46"/>
   </sortState>
-  <tableColumns count="15">
-    <tableColumn id="1" name="Status" dataDxfId="11"/>
-    <tableColumn id="2" name="Floor" dataDxfId="10"/>
-    <tableColumn id="16" name="Proxy" dataDxfId="9"/>
+  <tableColumns count="16">
+    <tableColumn id="1" name="Status" dataDxfId="12"/>
+    <tableColumn id="2" name="Floor" dataDxfId="11"/>
+    <tableColumn id="11" name="Modeled" dataDxfId="0"/>
+    <tableColumn id="16" name="Proxy" dataDxfId="10"/>
     <tableColumn id="3" name="Item"/>
-    <tableColumn id="4" name="Priority" dataDxfId="8"/>
-    <tableColumn id="15" name="Week" dataDxfId="7"/>
-    <tableColumn id="8" name="Time to spend" dataDxfId="6"/>
-    <tableColumn id="5" name="Poly " dataDxfId="5"/>
+    <tableColumn id="4" name="Priority" dataDxfId="9"/>
+    <tableColumn id="15" name="Week" dataDxfId="8"/>
+    <tableColumn id="8" name="Time to spend" dataDxfId="7"/>
+    <tableColumn id="5" name="Poly " dataDxfId="6"/>
     <tableColumn id="6" name="Texture"/>
     <tableColumn id="7" name="Model"/>
     <tableColumn id="9" name="References"/>
@@ -566,12 +573,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A52:C60" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A52:C60" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <autoFilter ref="A52:C60"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Week" dataDxfId="2"/>
-    <tableColumn id="2" name="Minutes" dataDxfId="1"/>
-    <tableColumn id="3" name="Hours" dataDxfId="0"/>
+    <tableColumn id="1" name="Week" dataDxfId="3"/>
+    <tableColumn id="2" name="Minutes" dataDxfId="2"/>
+    <tableColumn id="3" name="Hours" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -840,10 +847,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O59"/>
+  <dimension ref="A1:P59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -861,7 +868,7 @@
     <col min="11" max="11" width="26.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>57</v>
       </c>
@@ -869,46 +876,49 @@
         <v>58</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="J1" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -916,31 +926,34 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="1">
-        <v>1</v>
-      </c>
       <c r="F2" s="1">
         <v>1</v>
       </c>
       <c r="G2" s="1">
+        <v>1</v>
+      </c>
+      <c r="H2" s="1">
         <v>30</v>
       </c>
-      <c r="H2" s="1">
+      <c r="I2" s="1">
         <v>50</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>36</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="K2" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -948,31 +961,34 @@
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E3" t="s">
         <v>40</v>
       </c>
-      <c r="E3" s="1">
-        <v>1</v>
-      </c>
       <c r="F3" s="1">
         <v>1</v>
       </c>
       <c r="G3" s="1">
+        <v>1</v>
+      </c>
+      <c r="H3" s="1">
         <v>40</v>
       </c>
-      <c r="H3" s="1">
+      <c r="I3" s="1">
         <v>50</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>36</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="K3" s="4" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -980,31 +996,34 @@
         <v>28</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E4" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="1">
-        <v>1</v>
-      </c>
       <c r="F4" s="1">
         <v>1</v>
       </c>
       <c r="G4" s="1">
+        <v>1</v>
+      </c>
+      <c r="H4" s="1">
         <v>30</v>
       </c>
-      <c r="H4" s="1">
-        <v>1</v>
-      </c>
-      <c r="I4" t="s">
-        <v>38</v>
+      <c r="I4" s="1">
+        <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="K4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -1012,31 +1031,34 @@
         <v>2</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E5" t="s">
         <v>63</v>
       </c>
-      <c r="E5" s="1">
-        <v>1</v>
-      </c>
       <c r="F5" s="1">
         <v>1</v>
       </c>
       <c r="G5" s="1">
+        <v>1</v>
+      </c>
+      <c r="H5" s="1">
         <v>30</v>
       </c>
-      <c r="H5" s="1">
+      <c r="I5" s="1">
         <v>6</v>
       </c>
-      <c r="I5" t="s">
-        <v>38</v>
-      </c>
       <c r="J5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="K5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -1044,31 +1066,34 @@
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E6" t="s">
         <v>63</v>
       </c>
-      <c r="E6" s="1">
-        <v>1</v>
-      </c>
       <c r="F6" s="1">
         <v>1</v>
       </c>
       <c r="G6" s="1">
+        <v>1</v>
+      </c>
+      <c r="H6" s="1">
         <v>30</v>
       </c>
-      <c r="H6" s="1">
-        <v>1</v>
-      </c>
-      <c r="I6" t="s">
-        <v>38</v>
+      <c r="I6" s="1">
+        <v>1</v>
       </c>
       <c r="J6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="K6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
@@ -1076,31 +1101,34 @@
         <v>28</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E7" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="1">
-        <v>1</v>
-      </c>
       <c r="F7" s="1">
         <v>1</v>
       </c>
       <c r="G7" s="1">
+        <v>1</v>
+      </c>
+      <c r="H7" s="1">
         <v>30</v>
       </c>
-      <c r="H7" s="1">
-        <v>1</v>
-      </c>
-      <c r="I7" t="s">
-        <v>38</v>
+      <c r="I7" s="1">
+        <v>1</v>
       </c>
       <c r="J7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="K7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
@@ -1108,31 +1136,34 @@
         <v>28</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E8" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="1">
-        <v>1</v>
-      </c>
       <c r="F8" s="1">
         <v>1</v>
       </c>
       <c r="G8" s="1">
+        <v>1</v>
+      </c>
+      <c r="H8" s="1">
         <v>30</v>
       </c>
-      <c r="H8" s="1">
-        <v>1</v>
-      </c>
-      <c r="I8" t="s">
-        <v>38</v>
+      <c r="I8" s="1">
+        <v>1</v>
       </c>
       <c r="J8" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="K8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>3</v>
       </c>
@@ -1140,760 +1171,763 @@
         <v>1</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E9" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="1">
-        <v>1</v>
-      </c>
       <c r="F9" s="1">
         <v>1</v>
       </c>
       <c r="G9" s="1">
+        <v>1</v>
+      </c>
+      <c r="H9" s="1">
         <v>30</v>
       </c>
-      <c r="H9" s="1">
-        <v>1</v>
-      </c>
-      <c r="I9" t="s">
-        <v>38</v>
+      <c r="I9" s="1">
+        <v>1</v>
       </c>
       <c r="J9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="K9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="1">
         <v>1</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="D10" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E10" t="s">
         <v>88</v>
       </c>
-      <c r="E10" s="1">
-        <v>2</v>
-      </c>
       <c r="F10" s="1">
         <v>2</v>
       </c>
       <c r="G10" s="1">
+        <v>2</v>
+      </c>
+      <c r="H10" s="1">
         <v>30</v>
       </c>
-      <c r="H10" s="1">
+      <c r="I10" s="1">
         <v>50</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>65</v>
       </c>
-      <c r="J10" t="s">
+      <c r="K10" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="1">
         <v>1</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="D11" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E11" t="s">
         <v>87</v>
       </c>
-      <c r="E11" s="1">
-        <v>2</v>
-      </c>
       <c r="F11" s="1">
         <v>2</v>
       </c>
       <c r="G11" s="1">
+        <v>2</v>
+      </c>
+      <c r="H11" s="1">
         <v>30</v>
       </c>
-      <c r="H11" s="1">
+      <c r="I11" s="1">
         <v>50</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>65</v>
       </c>
-      <c r="J11" t="s">
+      <c r="K11" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B12" s="1">
         <v>2</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="D12" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E12" t="s">
         <v>32</v>
       </c>
-      <c r="E12" s="1">
-        <v>2</v>
-      </c>
       <c r="F12" s="1">
         <v>2</v>
       </c>
       <c r="G12" s="1">
+        <v>2</v>
+      </c>
+      <c r="H12" s="1">
         <v>30</v>
       </c>
-      <c r="H12" s="1">
+      <c r="I12" s="1">
         <v>50</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
         <v>65</v>
       </c>
-      <c r="J12" t="s">
+      <c r="K12" s="4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B13" s="1">
         <v>1</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="D13" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E13" t="s">
         <v>43</v>
       </c>
-      <c r="E13" s="1">
-        <v>2</v>
-      </c>
       <c r="F13" s="1">
         <v>2</v>
       </c>
       <c r="G13" s="1">
+        <v>2</v>
+      </c>
+      <c r="H13" s="1">
         <v>30</v>
       </c>
-      <c r="H13" s="1">
+      <c r="I13" s="1">
         <v>200</v>
       </c>
-      <c r="I13" t="s">
+      <c r="J13" t="s">
         <v>36</v>
       </c>
-      <c r="J13" t="s">
+      <c r="K13" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B14" s="1">
         <v>1</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D14" t="s">
+      <c r="D14" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E14" t="s">
         <v>85</v>
       </c>
-      <c r="E14" s="1">
-        <v>2</v>
-      </c>
       <c r="F14" s="1">
         <v>2</v>
       </c>
       <c r="G14" s="1">
+        <v>2</v>
+      </c>
+      <c r="H14" s="1">
         <v>30</v>
       </c>
-      <c r="H14" s="1">
+      <c r="I14" s="1">
         <v>50</v>
       </c>
-      <c r="I14" t="s">
+      <c r="J14" t="s">
         <v>42</v>
       </c>
-      <c r="J14" t="s">
-        <v>38</v>
-      </c>
       <c r="K14" t="s">
+        <v>38</v>
+      </c>
+      <c r="L14" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B15" s="1">
         <v>2</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D15" t="s">
+      <c r="D15" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E15" t="s">
         <v>47</v>
       </c>
-      <c r="E15" s="1">
-        <v>2</v>
-      </c>
       <c r="F15" s="1">
         <v>2</v>
       </c>
       <c r="G15" s="1">
+        <v>2</v>
+      </c>
+      <c r="H15" s="1">
         <v>40</v>
       </c>
-      <c r="H15" s="1">
+      <c r="I15" s="1">
         <v>50</v>
       </c>
-      <c r="I15" t="s">
+      <c r="J15" t="s">
         <v>68</v>
       </c>
-      <c r="J15" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B16" s="1">
         <v>1</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D16" t="s">
+      <c r="D16" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E16" t="s">
         <v>25</v>
       </c>
-      <c r="E16" s="1">
-        <v>2</v>
-      </c>
       <c r="F16" s="1">
         <v>2</v>
       </c>
       <c r="G16" s="1">
+        <v>2</v>
+      </c>
+      <c r="H16" s="1">
         <v>40</v>
       </c>
-      <c r="H16" s="1">
+      <c r="I16" s="1">
         <v>50</v>
       </c>
-      <c r="I16" t="s">
+      <c r="J16" t="s">
         <v>67</v>
       </c>
-      <c r="J16" t="s">
+      <c r="K16" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B17" s="1">
         <v>1</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D17" t="s">
+      <c r="D17" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E17" t="s">
         <v>9</v>
       </c>
-      <c r="E17" s="1">
-        <v>2</v>
-      </c>
       <c r="F17" s="1">
         <v>2</v>
       </c>
       <c r="G17" s="1">
+        <v>2</v>
+      </c>
+      <c r="H17" s="1">
         <v>100</v>
       </c>
-      <c r="H17" s="1">
+      <c r="I17" s="1">
         <v>250</v>
       </c>
-      <c r="I17" t="s">
+      <c r="J17" t="s">
         <v>67</v>
       </c>
-      <c r="J17" t="s">
+      <c r="K17" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B18" s="1">
         <v>1</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D18" t="s">
+      <c r="D18" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E18" t="s">
         <v>26</v>
       </c>
-      <c r="E18" s="1">
-        <v>2</v>
-      </c>
       <c r="F18" s="1">
         <v>2</v>
       </c>
       <c r="G18" s="1">
+        <v>2</v>
+      </c>
+      <c r="H18" s="1">
         <v>15</v>
       </c>
-      <c r="H18" s="1">
+      <c r="I18" s="1">
         <v>4</v>
       </c>
-      <c r="I18" t="s">
+      <c r="J18" t="s">
         <v>64</v>
       </c>
-      <c r="J18" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B19" s="1">
         <v>1</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D19" t="s">
+      <c r="D19" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E19" t="s">
         <v>11</v>
       </c>
-      <c r="E19" s="1">
-        <v>2</v>
-      </c>
       <c r="F19" s="1">
         <v>2</v>
       </c>
       <c r="G19" s="1">
+        <v>2</v>
+      </c>
+      <c r="H19" s="1">
         <v>60</v>
       </c>
-      <c r="H19" s="1">
+      <c r="I19" s="1">
         <v>400</v>
       </c>
-      <c r="I19" t="s">
-        <v>37</v>
-      </c>
       <c r="J19" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K19" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B20" s="1">
         <v>1</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D20" t="s">
+      <c r="D20" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E20" t="s">
         <v>89</v>
       </c>
-      <c r="E20" s="1">
+      <c r="F20" s="1">
         <v>4</v>
       </c>
-      <c r="F20" s="1">
-        <v>2</v>
-      </c>
       <c r="G20" s="1">
+        <v>2</v>
+      </c>
+      <c r="H20" s="1">
         <v>20</v>
       </c>
-      <c r="H20" s="1">
+      <c r="I20" s="1">
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D21" t="s">
+      <c r="D21" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E21" t="s">
         <v>29</v>
       </c>
-      <c r="E21" s="1">
-        <v>2</v>
-      </c>
       <c r="F21" s="1">
+        <v>2</v>
+      </c>
+      <c r="G21" s="1">
         <v>3</v>
       </c>
-      <c r="G21" s="1">
+      <c r="H21" s="1">
         <v>30</v>
       </c>
-      <c r="H21" s="1">
+      <c r="I21" s="1">
         <v>200</v>
       </c>
-      <c r="I21" t="s">
+      <c r="J21" t="s">
         <v>65</v>
       </c>
-      <c r="J21" t="s">
+      <c r="K21" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B22" s="1">
         <v>2</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D22" t="s">
+      <c r="D22" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E22" t="s">
         <v>27</v>
       </c>
-      <c r="E22" s="1">
+      <c r="F22" s="1">
         <v>8</v>
       </c>
-      <c r="F22" s="1">
+      <c r="G22" s="1">
         <v>3</v>
       </c>
-      <c r="G22" s="1">
+      <c r="H22" s="1">
         <v>15</v>
       </c>
-      <c r="H22" s="1">
+      <c r="I22" s="1">
         <v>400</v>
       </c>
-      <c r="I22" t="s">
-        <v>37</v>
-      </c>
       <c r="J22" t="s">
+        <v>37</v>
+      </c>
+      <c r="K22" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>56</v>
       </c>
       <c r="B23" s="1">
         <v>1</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D23" t="s">
+      <c r="D23" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E23" t="s">
         <v>84</v>
       </c>
-      <c r="E23" s="1">
-        <v>2</v>
-      </c>
       <c r="F23" s="1">
+        <v>2</v>
+      </c>
+      <c r="G23" s="1">
         <v>3</v>
       </c>
-      <c r="G23" s="1">
+      <c r="H23" s="1">
         <v>120</v>
       </c>
-      <c r="H23" s="1">
+      <c r="I23" s="1">
         <v>400</v>
       </c>
-      <c r="I23" t="s">
-        <v>38</v>
-      </c>
       <c r="J23" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>56</v>
       </c>
       <c r="B24" s="1">
         <v>1</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D24" t="s">
+      <c r="D24" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E24" t="s">
         <v>61</v>
       </c>
-      <c r="E24" s="1">
-        <v>2</v>
-      </c>
       <c r="F24" s="1">
+        <v>2</v>
+      </c>
+      <c r="G24" s="1">
         <v>3</v>
       </c>
-      <c r="G24" s="1">
+      <c r="H24" s="1">
         <v>120</v>
       </c>
-      <c r="H24" s="1">
+      <c r="I24" s="1">
         <v>400</v>
       </c>
-      <c r="I24" t="s">
-        <v>38</v>
-      </c>
-      <c r="J24" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J24" t="s">
+        <v>38</v>
+      </c>
+      <c r="K24" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>56</v>
       </c>
       <c r="B25" s="1">
         <v>1</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D25" t="s">
+      <c r="D25" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E25" t="s">
         <v>86</v>
       </c>
-      <c r="E25" s="1">
-        <v>2</v>
-      </c>
       <c r="F25" s="1">
+        <v>2</v>
+      </c>
+      <c r="G25" s="1">
         <v>3</v>
       </c>
-      <c r="G25" s="1">
+      <c r="H25" s="1">
         <v>120</v>
       </c>
-      <c r="H25" s="1">
+      <c r="I25" s="1">
         <v>400</v>
       </c>
-      <c r="I25" t="s">
-        <v>38</v>
-      </c>
       <c r="J25" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K25" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B26" s="1">
         <v>1</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D26" t="s">
+      <c r="D26" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E26" t="s">
         <v>12</v>
       </c>
-      <c r="E26" s="1">
-        <v>10</v>
-      </c>
       <c r="F26" s="1">
+        <v>10</v>
+      </c>
+      <c r="G26" s="1">
         <v>3</v>
       </c>
-      <c r="G26" s="1">
+      <c r="H26" s="1">
         <v>120</v>
       </c>
-      <c r="H26" s="1">
+      <c r="I26" s="1">
         <v>400</v>
       </c>
-      <c r="I26" t="s">
-        <v>38</v>
-      </c>
       <c r="J26" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K26" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B27" s="1">
         <v>1</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D27" t="s">
+      <c r="D27" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E27" t="s">
         <v>23</v>
-      </c>
-      <c r="E27" s="1">
-        <v>3</v>
       </c>
       <c r="F27" s="1">
         <v>3</v>
       </c>
       <c r="G27" s="1">
+        <v>3</v>
+      </c>
+      <c r="H27" s="1">
         <v>20</v>
       </c>
-      <c r="H27" s="1">
+      <c r="I27" s="1">
         <v>1000</v>
       </c>
-      <c r="I27" t="s">
-        <v>38</v>
-      </c>
       <c r="J27" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K27" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D28" t="s">
+      <c r="D28" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E28" t="s">
         <v>90</v>
       </c>
-      <c r="E28" s="1">
+      <c r="F28" s="1">
         <v>4</v>
       </c>
-      <c r="F28" s="1">
+      <c r="G28" s="1">
         <v>3</v>
       </c>
-      <c r="G28" s="1">
+      <c r="H28" s="1">
         <v>15</v>
       </c>
-      <c r="H28" s="1">
+      <c r="I28" s="1">
         <v>30</v>
       </c>
-      <c r="I28" t="s">
-        <v>38</v>
-      </c>
       <c r="J28" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K28" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D29" t="s">
+      <c r="D29" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E29" t="s">
         <v>13</v>
       </c>
-      <c r="E29" s="1">
+      <c r="F29" s="1">
         <v>4</v>
       </c>
-      <c r="F29" s="1">
+      <c r="G29" s="1">
         <v>3</v>
       </c>
-      <c r="G29" s="1">
+      <c r="H29" s="1">
         <v>30</v>
       </c>
-      <c r="H29" s="1">
+      <c r="I29" s="1">
         <v>100</v>
       </c>
-      <c r="I29" t="s">
-        <v>37</v>
-      </c>
       <c r="J29" t="s">
+        <v>37</v>
+      </c>
+      <c r="K29" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B30" s="1">
         <v>1</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D30" t="s">
+      <c r="D30" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E30" t="s">
         <v>14</v>
       </c>
-      <c r="E30" s="1">
+      <c r="F30" s="1">
         <v>4</v>
       </c>
-      <c r="F30" s="1">
+      <c r="G30" s="1">
         <v>3</v>
       </c>
-      <c r="G30" s="1">
+      <c r="H30" s="1">
         <v>30</v>
       </c>
-      <c r="H30" s="1">
+      <c r="I30" s="1">
         <v>100</v>
       </c>
-      <c r="I30" t="s">
-        <v>37</v>
-      </c>
       <c r="J30" t="s">
+        <v>37</v>
+      </c>
+      <c r="K30" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B31" s="1">
         <v>1</v>
       </c>
-      <c r="C31" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D31" t="s">
+      <c r="D31" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E31" t="s">
         <v>31</v>
       </c>
-      <c r="E31" s="1">
+      <c r="F31" s="1">
         <v>3</v>
       </c>
-      <c r="F31" s="1">
+      <c r="G31" s="1">
         <v>4</v>
       </c>
-      <c r="G31" s="1">
+      <c r="H31" s="1">
         <v>60</v>
       </c>
-      <c r="H31" s="1">
+      <c r="I31" s="1">
         <v>250</v>
       </c>
-      <c r="I31" t="s">
-        <v>37</v>
-      </c>
       <c r="J31" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K31" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B32" s="1">
         <v>1</v>
       </c>
-      <c r="C32" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D32" t="s">
+      <c r="D32" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E32" t="s">
         <v>24</v>
-      </c>
-      <c r="E32" s="1">
-        <v>3</v>
       </c>
       <c r="F32" s="1">
         <v>3</v>
       </c>
       <c r="G32" s="1">
+        <v>3</v>
+      </c>
+      <c r="H32" s="1">
         <v>30</v>
       </c>
-      <c r="H32" s="1">
+      <c r="I32" s="1">
         <v>300</v>
       </c>
-      <c r="I32" t="s">
-        <v>38</v>
-      </c>
       <c r="J32" t="s">
+        <v>38</v>
+      </c>
+      <c r="K32" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1904,25 +1938,26 @@
       <c r="B33" s="1">
         <v>1</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33" s="1"/>
+      <c r="E33" t="s">
         <v>15</v>
-      </c>
-      <c r="E33" s="1">
-        <v>4</v>
       </c>
       <c r="F33" s="1">
         <v>4</v>
       </c>
       <c r="G33" s="1">
+        <v>4</v>
+      </c>
+      <c r="H33" s="1">
         <v>60</v>
       </c>
-      <c r="H33" s="1">
+      <c r="I33" s="1">
         <v>6</v>
       </c>
-      <c r="I33" t="s">
-        <v>37</v>
-      </c>
       <c r="J33" t="s">
+        <v>37</v>
+      </c>
+      <c r="K33" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1933,28 +1968,28 @@
       <c r="B34" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C34" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D34" t="s">
+      <c r="D34" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E34" t="s">
         <v>21</v>
       </c>
-      <c r="E34" s="1">
+      <c r="F34" s="1">
         <v>12</v>
       </c>
-      <c r="F34" s="1">
+      <c r="G34" s="1">
         <v>4</v>
       </c>
-      <c r="G34" s="1">
+      <c r="H34" s="1">
         <v>15</v>
       </c>
-      <c r="H34" s="1">
+      <c r="I34" s="1">
         <v>30</v>
       </c>
-      <c r="I34" t="s">
-        <v>37</v>
-      </c>
       <c r="J34" t="s">
+        <v>37</v>
+      </c>
+      <c r="K34" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1965,28 +2000,28 @@
       <c r="B35" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C35" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D35" t="s">
+      <c r="D35" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E35" t="s">
         <v>16</v>
       </c>
-      <c r="E35" s="1">
+      <c r="F35" s="1">
         <v>12</v>
       </c>
-      <c r="F35" s="1">
+      <c r="G35" s="1">
         <v>4</v>
       </c>
-      <c r="G35" s="1">
+      <c r="H35" s="1">
         <v>15</v>
       </c>
-      <c r="H35" s="1">
+      <c r="I35" s="1">
         <v>20</v>
       </c>
-      <c r="I35" t="s">
-        <v>37</v>
-      </c>
       <c r="J35" t="s">
+        <v>37</v>
+      </c>
+      <c r="K35" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1997,28 +2032,28 @@
       <c r="B36" s="1">
         <v>1</v>
       </c>
-      <c r="C36" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D36" t="s">
+      <c r="D36" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E36" t="s">
         <v>78</v>
       </c>
-      <c r="E36" s="1">
+      <c r="F36" s="1">
         <v>15</v>
       </c>
-      <c r="F36" s="1">
+      <c r="G36" s="1">
         <v>4</v>
       </c>
-      <c r="G36" s="1">
+      <c r="H36" s="1">
         <v>30</v>
       </c>
-      <c r="H36" s="1">
+      <c r="I36" s="1">
         <v>200</v>
       </c>
-      <c r="I36" t="s">
-        <v>38</v>
-      </c>
-      <c r="J36" s="4" t="s">
+      <c r="J36" t="s">
+        <v>38</v>
+      </c>
+      <c r="K36" s="4" t="s">
         <v>79</v>
       </c>
     </row>
@@ -2029,28 +2064,28 @@
       <c r="B37" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C37" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D37" t="s">
+      <c r="D37" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E37" t="s">
         <v>20</v>
       </c>
-      <c r="E37" s="1">
+      <c r="F37" s="1">
         <v>12</v>
       </c>
-      <c r="F37" s="1">
+      <c r="G37" s="1">
         <v>4</v>
       </c>
-      <c r="G37" s="1">
+      <c r="H37" s="1">
         <v>15</v>
       </c>
-      <c r="H37" s="1">
-        <v>10</v>
-      </c>
-      <c r="I37" t="s">
-        <v>38</v>
+      <c r="I37" s="1">
+        <v>10</v>
       </c>
       <c r="J37" t="s">
+        <v>38</v>
+      </c>
+      <c r="K37" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2061,28 +2096,28 @@
       <c r="B38" s="1">
         <v>1</v>
       </c>
-      <c r="C38" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D38" t="s">
+      <c r="D38" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E38" t="s">
         <v>34</v>
       </c>
-      <c r="E38" s="1">
+      <c r="F38" s="1">
         <v>12</v>
       </c>
-      <c r="F38" s="1">
+      <c r="G38" s="1">
         <v>4</v>
       </c>
-      <c r="G38" s="1">
+      <c r="H38" s="1">
         <v>45</v>
       </c>
-      <c r="H38" s="1">
+      <c r="I38" s="1">
         <v>200</v>
       </c>
-      <c r="I38" t="s">
-        <v>38</v>
-      </c>
       <c r="J38" t="s">
+        <v>38</v>
+      </c>
+      <c r="K38" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2093,31 +2128,31 @@
       <c r="B39" s="1">
         <v>1</v>
       </c>
-      <c r="C39" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D39" t="s">
+      <c r="D39" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E39" t="s">
         <v>33</v>
       </c>
-      <c r="E39" s="1">
-        <v>10</v>
-      </c>
       <c r="F39" s="1">
+        <v>10</v>
+      </c>
+      <c r="G39" s="1">
         <v>4</v>
       </c>
-      <c r="G39" s="1">
+      <c r="H39" s="1">
         <v>120</v>
       </c>
-      <c r="H39" s="1">
+      <c r="I39" s="1">
         <v>400</v>
       </c>
-      <c r="I39" t="s">
-        <v>38</v>
-      </c>
       <c r="J39" t="s">
         <v>38</v>
       </c>
       <c r="K39" t="s">
+        <v>38</v>
+      </c>
+      <c r="L39" t="s">
         <v>71</v>
       </c>
     </row>
@@ -2128,25 +2163,26 @@
       <c r="B40" s="1">
         <v>2</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D40" s="1"/>
+      <c r="E40" t="s">
         <v>30</v>
       </c>
-      <c r="E40" s="1">
+      <c r="F40" s="1">
         <v>12</v>
       </c>
-      <c r="F40" s="1">
+      <c r="G40" s="1">
         <v>4</v>
       </c>
-      <c r="G40" s="1">
+      <c r="H40" s="1">
         <v>15</v>
       </c>
-      <c r="H40" s="1">
+      <c r="I40" s="1">
         <v>30</v>
       </c>
-      <c r="I40" t="s">
-        <v>38</v>
-      </c>
       <c r="J40" t="s">
+        <v>38</v>
+      </c>
+      <c r="K40" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2157,28 +2193,28 @@
       <c r="B41" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D41" t="s">
+      <c r="D41" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E41" t="s">
         <v>17</v>
       </c>
-      <c r="E41" s="1">
+      <c r="F41" s="1">
         <v>12</v>
       </c>
-      <c r="F41" s="1">
+      <c r="G41" s="1">
         <v>4</v>
       </c>
-      <c r="G41" s="1">
+      <c r="H41" s="1">
         <v>15</v>
       </c>
-      <c r="H41" s="1">
+      <c r="I41" s="1">
         <v>20</v>
       </c>
-      <c r="I41" t="s">
+      <c r="J41" t="s">
         <v>70</v>
       </c>
-      <c r="J41" t="s">
+      <c r="K41" t="s">
         <v>45</v>
       </c>
     </row>
@@ -2189,25 +2225,26 @@
       <c r="B42" s="1">
         <v>1</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D42" s="1"/>
+      <c r="E42" t="s">
         <v>22</v>
       </c>
-      <c r="E42" s="1">
+      <c r="F42" s="1">
         <v>15</v>
       </c>
-      <c r="F42" s="1">
+      <c r="G42" s="1">
         <v>4</v>
       </c>
-      <c r="G42" s="1">
+      <c r="H42" s="1">
         <v>30</v>
       </c>
-      <c r="H42" s="1">
+      <c r="I42" s="1">
         <v>150</v>
       </c>
-      <c r="I42" t="s">
-        <v>38</v>
-      </c>
       <c r="J42" t="s">
+        <v>38</v>
+      </c>
+      <c r="K42" t="s">
         <v>77</v>
       </c>
     </row>
@@ -2218,28 +2255,28 @@
       <c r="B43" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C43" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D43" t="s">
+      <c r="D43" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E43" t="s">
         <v>19</v>
       </c>
-      <c r="E43" s="1">
+      <c r="F43" s="1">
         <v>12</v>
       </c>
-      <c r="F43" s="1">
+      <c r="G43" s="1">
         <v>4</v>
       </c>
-      <c r="G43" s="1">
+      <c r="H43" s="1">
         <v>30</v>
       </c>
-      <c r="H43" s="1">
+      <c r="I43" s="1">
         <v>20</v>
       </c>
-      <c r="I43" t="s">
-        <v>37</v>
-      </c>
       <c r="J43" t="s">
+        <v>37</v>
+      </c>
+      <c r="K43" t="s">
         <v>37</v>
       </c>
     </row>
@@ -2250,30 +2287,40 @@
       <c r="B44" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C44" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D44" t="s">
+      <c r="D44" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E44" t="s">
         <v>18</v>
       </c>
-      <c r="E44" s="1">
+      <c r="F44" s="1">
         <v>12</v>
       </c>
-      <c r="F44" s="1">
+      <c r="G44" s="1">
         <v>4</v>
       </c>
-      <c r="G44" s="1">
+      <c r="H44" s="1">
         <v>30</v>
       </c>
-      <c r="H44" s="1">
+      <c r="I44" s="1">
         <v>20</v>
       </c>
-      <c r="I44" t="s">
-        <v>38</v>
-      </c>
       <c r="J44" t="s">
-        <v>37</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="K44" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D45" s="1"/>
+      <c r="E45"/>
+      <c r="I45" s="1"/>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D46" s="1"/>
+      <c r="E46"/>
+      <c r="I46" s="1"/>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
@@ -2285,11 +2332,11 @@
       <c r="E48" s="6"/>
       <c r="F48" s="6"/>
       <c r="G48" s="6">
-        <f>SUM(G2:G46)</f>
+        <f>SUM(H2:H46)</f>
         <v>1805</v>
       </c>
       <c r="H48" s="6">
-        <f>SUM(H2:H46)</f>
+        <f>SUM(I2:I46)</f>
         <v>6401</v>
       </c>
       <c r="I48" s="7"/>
@@ -2321,7 +2368,7 @@
         <v>35</v>
       </c>
       <c r="B53" s="1">
-        <f>SUM(G2:G46)</f>
+        <f>SUM(H2:H46)</f>
         <v>1805</v>
       </c>
       <c r="C53" s="1">
@@ -2409,16 +2456,17 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J36" r:id="rId1"/>
-    <hyperlink ref="J2" r:id="rId2"/>
-    <hyperlink ref="J3" r:id="rId3"/>
+    <hyperlink ref="K36" r:id="rId1"/>
+    <hyperlink ref="K2" r:id="rId2"/>
+    <hyperlink ref="K3" r:id="rId3"/>
+    <hyperlink ref="K12" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
-  <drawing r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
+  <drawing r:id="rId6"/>
   <tableParts count="2">
-    <tablePart r:id="rId6"/>
     <tablePart r:id="rId7"/>
+    <tablePart r:id="rId8"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>